<commit_message>
Properties Listed and Hash registered
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software Codes\FYP\NFT_Fractionalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0F28A4-C7EE-49E4-9CD3-AEF6E288650B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF8E4F-7761-4FC9-BB59-ACCE5B439DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>07bac3f92e7fb49f1698f00d9648bd97911bbb18431f212141caa3890f907939</t>
   </si>
@@ -35,18 +35,30 @@
   <si>
     <t>07bacqwewqewqewq3f92e7fb49f1698f00d9648bd97911bbb18431f212141caa3890f907939</t>
   </si>
+  <si>
+    <t>aabfebe72a7b7e802fc567d097979e1f728df9956b9e522016fef04903af903e</t>
+  </si>
+  <si>
+    <t>19b0a0ce0dbfa2a6403592fffdf8c30587c6fbc78dae5eafa9ff803829b081c3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -374,6 +387,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
init laptop change final
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software Codes\FYP\NFT_Fractionalization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAF8E4F-7761-4FC9-BB59-ACCE5B439DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF6D373-03A3-4354-B79B-31B682D65089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>07bac3f92e7fb49f1698f00d9648bd97911bbb18431f212141caa3890f907939</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>19b0a0ce0dbfa2a6403592fffdf8c30587c6fbc78dae5eafa9ff803829b081c3</t>
+  </si>
+  <si>
+    <t>8cdc5e926dfa8ac66d777503aaa28b7085e76b7c12e32dc7b7a578bc4892dea9</t>
+  </si>
+  <si>
+    <t>3fbdafef1da1e7d10382fabfaec7d5980e9f6c765b953f5ba9e028d0c884f6d6</t>
   </si>
 </sst>
 </file>
@@ -364,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,6 +403,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>